<commit_message>
changes to Grid and Logs
</commit_message>
<xml_diff>
--- a/COMP3004_Game_Iteration01/Game/SetupGame/Logs/grid_Team03.xlsx
+++ b/COMP3004_Game_Iteration01/Game/SetupGame/Logs/grid_Team03.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AlfrancisStudent/Documents/Object Oriented Programming/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heewo\Documents\ComputerScience\3004\FirstIteration\QuestOfTheRoundTable\COMP3004_Game_Iteration01\Game\SetupGame\Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C5CB27-D8E7-40BD-8A43-94DF44B687E5}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="111">
   <si>
     <t>is it possible for a participant to NOT play a card for a stage</t>
     <phoneticPr fontId="6" type="noConversion"/>
@@ -355,13 +356,25 @@
   </si>
   <si>
     <t>EventsAndAllyLog.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cannot be discarded </t>
+  </si>
+  <si>
+    <t>cards are added right away after submitted</t>
+  </si>
+  <si>
+    <t>QuestLog.txt</t>
+  </si>
+  <si>
+    <t>QuestAndEventsLog</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -420,16 +433,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF333333"/>
       <name val="Menlo"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -565,6 +579,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -891,38 +908,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="80.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
-    <col min="4" max="4" width="24.1640625" customWidth="1"/>
+    <col min="2" max="2" width="11.6484375" customWidth="1"/>
+    <col min="4" max="4" width="24.1484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>91</v>
       </c>
       <c r="B2" s="5"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>92</v>
       </c>
       <c r="B3" s="5"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="B4" s="5" t="s">
         <v>56</v>
       </c>
@@ -933,20 +950,20 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>65</v>
       </c>
@@ -960,7 +977,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -974,7 +991,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -985,7 +1002,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>61</v>
       </c>
@@ -996,7 +1013,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -1010,7 +1027,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -1024,7 +1041,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -1038,7 +1055,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -1052,7 +1069,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>63</v>
       </c>
@@ -1063,7 +1080,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>64</v>
       </c>
@@ -1077,7 +1094,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>67</v>
       </c>
@@ -1091,7 +1108,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>66</v>
       </c>
@@ -1105,7 +1122,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>68</v>
       </c>
@@ -1119,340 +1136,428 @@
         <v>101</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>71</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>70</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>73</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>72</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>44</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>74</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>47</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B35" s="3"/>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>50</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>0</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D37" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="6" t="s">
         <v>94</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>2</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D39" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>75</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D40" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>51</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D41" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>52</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D42" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
         <v>53</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D43" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
         <v>54</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D44" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
         <v>55</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D45" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" t="s">
         <v>33</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B46" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D46" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" t="s">
         <v>34</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B47" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D47" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" t="s">
         <v>35</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="B48" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D48" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" t="s">
         <v>36</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="B49" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>59</v>
       </c>
+      <c r="D49" t="s">
+        <v>109</v>
+      </c>
       <c r="G49" s="1"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7">
+      <c r="B50" s="3"/>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="B51" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D51" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52" s="1"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7">
       <c r="A54" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7">
       <c r="A55" t="s">
         <v>77</v>
       </c>
@@ -1463,7 +1568,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7">
       <c r="A56" s="3" t="s">
         <v>29</v>
       </c>
@@ -1474,7 +1579,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7">
       <c r="A57" s="3" t="s">
         <v>30</v>
       </c>
@@ -1485,7 +1590,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7">
       <c r="A58" s="3" t="s">
         <v>15</v>
       </c>
@@ -1497,7 +1602,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7">
       <c r="A59" t="s">
         <v>16</v>
       </c>
@@ -1508,7 +1613,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7">
       <c r="A60" t="s">
         <v>17</v>
       </c>
@@ -1519,18 +1624,18 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7">
       <c r="A61" t="s">
         <v>18</v>
       </c>
-      <c r="B61" s="6" t="s">
-        <v>94</v>
+      <c r="B61" s="6">
+        <v>0</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7">
       <c r="A62" s="3" t="s">
         <v>14</v>
       </c>
@@ -1541,7 +1646,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7">
       <c r="A63" s="3" t="s">
         <v>79</v>
       </c>
@@ -1552,21 +1657,21 @@
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4">
       <c r="A65" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4">
       <c r="A66" s="4" t="s">
         <v>80</v>
       </c>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4">
       <c r="A67" t="s">
         <v>5</v>
       </c>
@@ -1580,11 +1685,11 @@
         <v>104</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4">
       <c r="A68" t="s">
         <v>81</v>
       </c>
-      <c r="B68" s="8">
+      <c r="B68" s="7">
         <v>2</v>
       </c>
       <c r="C68" s="6" t="s">
@@ -1594,7 +1699,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4">
       <c r="A69" t="s">
         <v>6</v>
       </c>
@@ -1608,7 +1713,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4">
       <c r="A70" t="s">
         <v>7</v>
       </c>
@@ -1622,11 +1727,11 @@
         <v>106</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4">
       <c r="A71" t="s">
         <v>8</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B71" s="8" t="s">
         <v>93</v>
       </c>
       <c r="C71" t="s">
@@ -1636,63 +1741,74 @@
         <v>106</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4">
       <c r="A72" t="s">
         <v>9</v>
       </c>
-      <c r="B72" s="3" t="s">
-        <v>94</v>
+      <c r="B72" s="8" t="s">
+        <v>93</v>
       </c>
       <c r="C72" t="s">
         <v>59</v>
       </c>
-      <c r="D72" s="6"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D72" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
       <c r="A73" t="s">
         <v>10</v>
       </c>
-      <c r="B73" s="3" t="s">
-        <v>94</v>
+      <c r="B73" s="8" t="s">
+        <v>93</v>
       </c>
       <c r="C73" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D73" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
       <c r="A74" t="s">
         <v>11</v>
       </c>
-      <c r="B74" t="s">
-        <v>94</v>
+      <c r="B74" s="8" t="s">
+        <v>93</v>
       </c>
       <c r="C74" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D74" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
       <c r="A75" t="s">
         <v>12</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="3" t="s">
         <v>94</v>
       </c>
       <c r="C75" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4">
       <c r="A76" t="s">
         <v>13</v>
       </c>
-      <c r="B76" t="s">
-        <v>94</v>
+      <c r="B76" s="8" t="s">
+        <v>93</v>
       </c>
       <c r="C76" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D76" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
       <c r="A78" t="s">
         <v>82</v>
       </c>
@@ -1703,7 +1819,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4">
       <c r="A79" t="s">
         <v>20</v>
       </c>
@@ -1714,34 +1830,34 @@
         <v>59</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4">
       <c r="A81" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4">
       <c r="A82" t="s">
         <v>83</v>
       </c>
-      <c r="B82" s="7" t="s">
+      <c r="B82" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C82" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4">
       <c r="A83" t="s">
         <v>21</v>
       </c>
-      <c r="B83" s="7" t="s">
+      <c r="B83" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C83" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4">
       <c r="A85" t="s">
         <v>23</v>
       </c>
@@ -1755,7 +1871,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4">
       <c r="A87" t="s">
         <v>26</v>
       </c>
@@ -1766,7 +1882,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4">
       <c r="A88" t="s">
         <v>27</v>
       </c>
@@ -1777,14 +1893,14 @@
         <v>59</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4">
       <c r="A90" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4">
       <c r="A91" t="s">
         <v>84</v>
       </c>
@@ -1795,28 +1911,31 @@
         <v>59</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4">
       <c r="A92" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4">
       <c r="A93" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4">
       <c r="A94" t="s">
         <v>3</v>
       </c>
-      <c r="B94" s="6" t="s">
-        <v>94</v>
+      <c r="B94" s="8" t="s">
+        <v>93</v>
       </c>
       <c r="C94" s="6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D94" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
       <c r="A95" t="s">
         <v>25</v>
       </c>
@@ -1827,7 +1946,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3">
       <c r="A97" t="s">
         <v>88</v>
       </c>
@@ -1835,17 +1954,17 @@
         <v>87</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3">
       <c r="A100" s="5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3">
       <c r="A101" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3">
       <c r="A102" t="s">
         <v>95</v>
       </c>
@@ -1856,7 +1975,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3">
       <c r="A103" t="s">
         <v>96</v>
       </c>
@@ -1867,7 +1986,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3">
       <c r="A104" t="s">
         <v>97</v>
       </c>
@@ -1878,7 +1997,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3">
       <c r="A105" t="s">
         <v>98</v>
       </c>
@@ -1892,6 +2011,6 @@
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>